<commit_message>
maintenance - fixed various issues
</commit_message>
<xml_diff>
--- a/tests/input/sample.xlsx
+++ b/tests/input/sample.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23515"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="57440" yWindow="2840" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="9580" yWindow="4940" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="914" uniqueCount="768">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="932" uniqueCount="786">
   <si>
     <t>Some text</t>
   </si>
@@ -3138,6 +3138,60 @@
   </si>
   <si>
     <t>Boolean</t>
+  </si>
+  <si>
+    <t>Random1</t>
+  </si>
+  <si>
+    <t>Random2</t>
+  </si>
+  <si>
+    <t>Random3</t>
+  </si>
+  <si>
+    <t>Random4</t>
+  </si>
+  <si>
+    <t>Random5</t>
+  </si>
+  <si>
+    <t>Random6</t>
+  </si>
+  <si>
+    <t>Random7</t>
+  </si>
+  <si>
+    <t>Random8</t>
+  </si>
+  <si>
+    <t>Random9</t>
+  </si>
+  <si>
+    <t>Random10</t>
+  </si>
+  <si>
+    <t>Random11</t>
+  </si>
+  <si>
+    <t>Random12</t>
+  </si>
+  <si>
+    <t>Random13</t>
+  </si>
+  <si>
+    <t>Random14</t>
+  </si>
+  <si>
+    <t>Random15</t>
+  </si>
+  <si>
+    <t>Random16</t>
+  </si>
+  <si>
+    <t>Random17</t>
+  </si>
+  <si>
+    <t>Random18</t>
   </si>
 </sst>
 </file>
@@ -3643,10 +3697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:Z51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3658,7 +3712,7 @@
     <col min="5" max="5" width="11.6640625" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:26">
       <c r="A1" s="2" t="s">
         <v>5</v>
       </c>
@@ -3683,8 +3737,62 @@
       <c r="H1" s="2" t="s">
         <v>767</v>
       </c>
-    </row>
-    <row r="2" spans="1:8">
+      <c r="I1" s="2" t="s">
+        <v>768</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>769</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>770</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>771</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>772</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>773</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>774</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>775</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>776</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>777</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>778</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>780</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>781</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>782</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>783</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>784</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3708,8 +3816,80 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:8">
+      <c r="I2">
+        <f ca="1">RAND()</f>
+        <v>0.49864331231610581</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:Z16" ca="1" si="0">RAND()</f>
+        <v>1.7281426290981616E-2</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.4143345167932454</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.14781785072917464</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.0607503931618725E-2</v>
+      </c>
+      <c r="N2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.6555383852823421</v>
+      </c>
+      <c r="O2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.25623406527759951</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.25759222021646577</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.73122448996199141</v>
+      </c>
+      <c r="R2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.20211535987183915</v>
+      </c>
+      <c r="S2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.61249250465655725</v>
+      </c>
+      <c r="T2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.52967076256098966</v>
+      </c>
+      <c r="U2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.61445925963885817</v>
+      </c>
+      <c r="V2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.3374497097732394</v>
+      </c>
+      <c r="W2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.94945673959848298</v>
+      </c>
+      <c r="X2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.66368972794249448</v>
+      </c>
+      <c r="Y2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.85105195727410732</v>
+      </c>
+      <c r="Z2">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.15629839287504532</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3733,8 +3913,80 @@
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="I3">
+        <f t="shared" ref="I3:X34" ca="1" si="1">RAND()</f>
+        <v>0.76128678235704894</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.99772646770458606</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.33959387856405532</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.5411776591449784</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.39523229145574679</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.91618371790176156</v>
+      </c>
+      <c r="O3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.17381363532221294</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.50255868025288197</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.60418612609183531</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.22118986669169682</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.3880237539857831E-2</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.84902888852116731</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.88962757542868465</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.55086195501175617</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.58708937645775994</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.58234484466583059</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.50923660730440645</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.86039061548694562</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4">
         <v>3</v>
       </c>
@@ -3758,8 +4010,80 @@
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="I4">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.63911490119944914</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.4287005663360404E-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.55760296445790047</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.43319897263280538</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.6096713375276535E-3</v>
+      </c>
+      <c r="N4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.25040554183141139</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.80810408035391723</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.11010374422258107</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.89577925898627286</v>
+      </c>
+      <c r="R4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.25280939559512305</v>
+      </c>
+      <c r="S4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.89142208905736131</v>
+      </c>
+      <c r="T4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.35485227013908849</v>
+      </c>
+      <c r="U4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.34565084734236784</v>
+      </c>
+      <c r="V4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.65818321497558463</v>
+      </c>
+      <c r="W4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.46665591728392231</v>
+      </c>
+      <c r="X4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.7889783406197548</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.1296678102666933E-2</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.95200600004740887</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5">
         <v>4</v>
       </c>
@@ -3776,15 +4100,87 @@
         <v>41278</v>
       </c>
       <c r="G5" t="e">
-        <f t="shared" ref="G5:G51" si="0">1/0</f>
+        <f t="shared" ref="G5" si="2">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H5" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="I5">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.50150611052875627</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.56511753292768652</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.38808299570430771</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.83039166978393986</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.72934106364204576</v>
+      </c>
+      <c r="N5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.72901116926480669</v>
+      </c>
+      <c r="O5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.59193604903640096</v>
+      </c>
+      <c r="P5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.50621472668620415</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.8358319191179731E-2</v>
+      </c>
+      <c r="R5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.44884031831588234</v>
+      </c>
+      <c r="S5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.59998144242645979</v>
+      </c>
+      <c r="T5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.55544887489887951</v>
+      </c>
+      <c r="U5">
+        <f t="shared" ca="1" si="0"/>
+        <v>8.8820231496460011E-2</v>
+      </c>
+      <c r="V5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.20853093525215027</v>
+      </c>
+      <c r="W5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.58195545717744612</v>
+      </c>
+      <c r="X5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.48684873126402417</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.20472047477743005</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.8121975799509884</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6">
         <v>5</v>
       </c>
@@ -3801,15 +4197,87 @@
         <v>41279.666666666664</v>
       </c>
       <c r="G6" t="e">
-        <f t="shared" ref="G6:G51" si="1">something</f>
+        <f t="shared" ref="G6" si="3">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H6" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="I6">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.3092910889255256E-3</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.58253911054125063</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.80945286937916927</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.71111503421688482</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.65305177868999098</v>
+      </c>
+      <c r="N6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.97109631394363305</v>
+      </c>
+      <c r="O6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.38606682858390851</v>
+      </c>
+      <c r="P6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.55268386837542383</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.30439395376294442</v>
+      </c>
+      <c r="R6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.69154102998774991</v>
+      </c>
+      <c r="S6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.57229118546169599</v>
+      </c>
+      <c r="T6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.97973916617852974</v>
+      </c>
+      <c r="U6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1396279161113021</v>
+      </c>
+      <c r="V6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.83485309050262224</v>
+      </c>
+      <c r="W6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.81856429964457933</v>
+      </c>
+      <c r="X6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.6254194994215333</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.50429986929750636</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.41132075256120793</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7">
         <v>6</v>
       </c>
@@ -3826,15 +4294,87 @@
         <v>41275.537743055553</v>
       </c>
       <c r="G7" t="e">
-        <f t="shared" ref="G7:G51" si="2">"abc"+1</f>
+        <f t="shared" ref="G7" si="4">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H7" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="I7">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.6457597648505482</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.22618377910534715</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.17518902147475668</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.83326513368540711</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10480125322346845</v>
+      </c>
+      <c r="N7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.95428290018619411</v>
+      </c>
+      <c r="O7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.23727580727452691</v>
+      </c>
+      <c r="P7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.71337217981690393</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.20763462298971624</v>
+      </c>
+      <c r="R7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.87180789294564076</v>
+      </c>
+      <c r="S7">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.5075954536346514E-2</v>
+      </c>
+      <c r="T7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.23024012130534566</v>
+      </c>
+      <c r="U7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.47283668812998436</v>
+      </c>
+      <c r="V7">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.4108161386670637E-2</v>
+      </c>
+      <c r="W7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.3811427983903809</v>
+      </c>
+      <c r="X7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.18161366315039484</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.37461947858598266</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.9026477873648324E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3851,15 +4391,87 @@
         <v>3.9351851851851852E-4</v>
       </c>
       <c r="G8" t="e">
-        <f t="shared" ref="G8:G51" si="3">1/0</f>
+        <f t="shared" ref="G8" si="5">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H8" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="I8">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.4096837510483482</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.14055889332987925</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.65680251527267652</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.71542974162745965</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.36364807039299019</v>
+      </c>
+      <c r="N8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.74585379599162061</v>
+      </c>
+      <c r="O8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.69614085331694664</v>
+      </c>
+      <c r="P8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.74079238156941352</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.88157200446769746</v>
+      </c>
+      <c r="R8">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.0559469423754786E-2</v>
+      </c>
+      <c r="S8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.65576821257556928</v>
+      </c>
+      <c r="T8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.26531002659208236</v>
+      </c>
+      <c r="U8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10854633820932202</v>
+      </c>
+      <c r="V8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.26818341036692683</v>
+      </c>
+      <c r="W8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.68037907686381816</v>
+      </c>
+      <c r="X8">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.6753813152206827E-2</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.24888903977578547</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.15868345440357923</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3876,15 +4488,87 @@
         <v>41277.156481481485</v>
       </c>
       <c r="G9" t="e">
-        <f t="shared" ref="G9:G51" si="4">something</f>
+        <f t="shared" ref="G9" si="6">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H9" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="I9">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.26085102078688349</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.28723816385285206</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.58222741200148076</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.9129466332230417</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.38839496895024439</v>
+      </c>
+      <c r="N9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.35346218086796777</v>
+      </c>
+      <c r="O9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.81905567970203719</v>
+      </c>
+      <c r="P9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.5532407379255383</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.9073457884275119</v>
+      </c>
+      <c r="R9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.46422784974189879</v>
+      </c>
+      <c r="S9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.26093786623974391</v>
+      </c>
+      <c r="T9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.63224278186584559</v>
+      </c>
+      <c r="U9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.86304817813130597</v>
+      </c>
+      <c r="V9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.51370756865586897</v>
+      </c>
+      <c r="W9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.38651799569111134</v>
+      </c>
+      <c r="X9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.74042190201857472</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.0307510421598756E-2</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.34274341194465541</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3901,15 +4585,87 @@
         <v>41278</v>
       </c>
       <c r="G10" t="e">
-        <f t="shared" ref="G10:G51" si="5">"abc"+1</f>
+        <f t="shared" ref="G10" si="7">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H10" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="I10">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.49331874132581299</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.62145574445958074</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.34290461098373748</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.9240785423739144</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.62020749017891563</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.68798839100790854</v>
+      </c>
+      <c r="O10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.5638959519779817</v>
+      </c>
+      <c r="P10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.22225409714688726</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.82463042239970097</v>
+      </c>
+      <c r="R10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.66326524833575307</v>
+      </c>
+      <c r="S10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.49249347585499115</v>
+      </c>
+      <c r="T10">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.6108368429120778E-3</v>
+      </c>
+      <c r="U10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.78155444443960254</v>
+      </c>
+      <c r="V10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.34437150299398023</v>
+      </c>
+      <c r="W10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.51262564825263324</v>
+      </c>
+      <c r="X10">
+        <f t="shared" ca="1" si="0"/>
+        <v>2.7312994345289554E-2</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.69337645542858461</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1517816935561086</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11">
         <v>10</v>
       </c>
@@ -3926,15 +4682,87 @@
         <v>41279.666666666664</v>
       </c>
       <c r="G11" t="e">
-        <f t="shared" ref="G11:G51" si="6">1/0</f>
+        <f t="shared" ref="G11" si="8">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H11" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="I11">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.55486651078309768</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.69984988496823353</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.67467260412328944</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.68017206505641992</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1036806404064633</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.9417170880006791</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.92037355825893075</v>
+      </c>
+      <c r="P11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.37048577794728399</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.2846264127137434E-2</v>
+      </c>
+      <c r="R11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.48586399558947324</v>
+      </c>
+      <c r="S11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.17625517961914172</v>
+      </c>
+      <c r="T11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.31019132802819938</v>
+      </c>
+      <c r="U11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.71096556672995759</v>
+      </c>
+      <c r="V11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.14593294257056222</v>
+      </c>
+      <c r="W11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10296439044096706</v>
+      </c>
+      <c r="X11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.80895280323838414</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.99104519094345456</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.8788179613340783E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12">
         <v>11</v>
       </c>
@@ -3951,15 +4779,87 @@
         <v>41275.537743055553</v>
       </c>
       <c r="G12" t="e">
-        <f t="shared" ref="G12:G51" si="7">something</f>
+        <f t="shared" ref="G12" si="9">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H12" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="I12">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.83985848653437767</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.59474894350872742</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.6628378284136871</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.45686354020504227</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.64211699788612353</v>
+      </c>
+      <c r="N12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.42161769717503206</v>
+      </c>
+      <c r="O12">
+        <f t="shared" ca="1" si="0"/>
+        <v>7.6469863387106041E-2</v>
+      </c>
+      <c r="P12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.82507928736579039</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.55915865691764077</v>
+      </c>
+      <c r="R12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.59661921899072834</v>
+      </c>
+      <c r="S12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.83617186303054791</v>
+      </c>
+      <c r="T12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.95839856310762195</v>
+      </c>
+      <c r="U12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.57894961514255872</v>
+      </c>
+      <c r="V12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.16859698123284406</v>
+      </c>
+      <c r="W12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.99639889433406592</v>
+      </c>
+      <c r="X12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.90703303060548546</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.99388919015039834</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.97181928821820929</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13">
         <v>12</v>
       </c>
@@ -3976,15 +4876,87 @@
         <v>3.9351851851851852E-4</v>
       </c>
       <c r="G13" t="e">
-        <f t="shared" ref="G13:G51" si="8">"abc"+1</f>
+        <f t="shared" ref="G13" si="10">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H13" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="I13">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.780126662292969E-2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.45865686030738795</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ca="1" si="0"/>
+        <v>3.163624396335607E-2</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.13490551904561143</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.86043199079762545</v>
+      </c>
+      <c r="N13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.87250210302797349</v>
+      </c>
+      <c r="O13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.30720331084835972</v>
+      </c>
+      <c r="P13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.28538782547369757</v>
+      </c>
+      <c r="Q13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.34411617559496865</v>
+      </c>
+      <c r="R13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.97921831400794468</v>
+      </c>
+      <c r="S13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.43598049370697944</v>
+      </c>
+      <c r="T13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.58308398840426134</v>
+      </c>
+      <c r="U13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.20809150543923915</v>
+      </c>
+      <c r="V13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.35476170329449863</v>
+      </c>
+      <c r="W13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.75307595967181262</v>
+      </c>
+      <c r="X13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.69479008257624486</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.16009189684250358</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.30680746548829807</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26">
       <c r="A14">
         <v>13</v>
       </c>
@@ -4001,15 +4973,87 @@
         <v>41277.156481481485</v>
       </c>
       <c r="G14" t="e">
-        <f t="shared" ref="G14:G51" si="9">1/0</f>
+        <f t="shared" ref="G14" si="11">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H14" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:8">
+      <c r="I14">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.42400444490007017</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.71437827921451669</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.27210362503329677</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.41499008902920353</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.35619899751694284</v>
+      </c>
+      <c r="N14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.51424037357377717</v>
+      </c>
+      <c r="O14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.35975618268427922</v>
+      </c>
+      <c r="P14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.26705905094133509</v>
+      </c>
+      <c r="Q14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.50506292090418725</v>
+      </c>
+      <c r="R14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.39591361240341361</v>
+      </c>
+      <c r="S14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.95070925459499378</v>
+      </c>
+      <c r="T14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.26488528253074706</v>
+      </c>
+      <c r="U14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.49393999873915906</v>
+      </c>
+      <c r="V14">
+        <f t="shared" ca="1" si="0"/>
+        <v>4.8451046751562754E-2</v>
+      </c>
+      <c r="W14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.51261754056242481</v>
+      </c>
+      <c r="X14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.69694199836738902</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.9767325210114175</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.82021464804026778</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26">
       <c r="A15">
         <v>14</v>
       </c>
@@ -4026,15 +5070,87 @@
         <v>41278</v>
       </c>
       <c r="G15" t="e">
-        <f t="shared" ref="G15:G51" si="10">something</f>
+        <f t="shared" ref="G15" si="12">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H15" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:8">
+      <c r="I15">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.34944185651869797</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.14324556884248452</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.22475484061455764</v>
+      </c>
+      <c r="L15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.66803764805240362</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ca="1" si="0"/>
+        <v>6.8962215355527379E-2</v>
+      </c>
+      <c r="N15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.95304224434373752</v>
+      </c>
+      <c r="O15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.84164139054870768</v>
+      </c>
+      <c r="P15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.76113843413268645</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.46445168560172057</v>
+      </c>
+      <c r="R15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.53324189955846923</v>
+      </c>
+      <c r="S15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.10704754703783737</v>
+      </c>
+      <c r="T15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.73405282987535903</v>
+      </c>
+      <c r="U15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.54485257001354437</v>
+      </c>
+      <c r="V15">
+        <f t="shared" ca="1" si="0"/>
+        <v>1.7913048654433772E-2</v>
+      </c>
+      <c r="W15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.31547809618580724</v>
+      </c>
+      <c r="X15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.68157416092473455</v>
+      </c>
+      <c r="Y15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.28855165737563349</v>
+      </c>
+      <c r="Z15">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.29290110796505564</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16">
         <v>15</v>
       </c>
@@ -4051,15 +5167,87 @@
         <v>41279.666666666664</v>
       </c>
       <c r="G16" t="e">
-        <f t="shared" ref="G16:G51" si="11">"abc"+1</f>
+        <f t="shared" ref="G16" si="13">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H16" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:8">
+      <c r="I16">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.46367932278575352</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.64663953326410462</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.4909678691786894</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.24857530438236253</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.407342685601915</v>
+      </c>
+      <c r="N16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.17096918163804753</v>
+      </c>
+      <c r="O16">
+        <f t="shared" ca="1" si="0"/>
+        <v>5.4960102666532507E-3</v>
+      </c>
+      <c r="P16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.15092567762770759</v>
+      </c>
+      <c r="Q16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.96244745920299701</v>
+      </c>
+      <c r="R16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.29227905222984152</v>
+      </c>
+      <c r="S16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.41891716081118535</v>
+      </c>
+      <c r="T16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.40739977468084398</v>
+      </c>
+      <c r="U16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.86133012915784057</v>
+      </c>
+      <c r="V16">
+        <f t="shared" ca="1" si="0"/>
+        <v>9.4570706628739121E-2</v>
+      </c>
+      <c r="W16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.1001301759921559</v>
+      </c>
+      <c r="X16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.90860857427038322</v>
+      </c>
+      <c r="Y16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.7174150013361178</v>
+      </c>
+      <c r="Z16">
+        <f t="shared" ca="1" si="0"/>
+        <v>0.65673614838238714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26">
       <c r="A17">
         <v>16</v>
       </c>
@@ -4076,15 +5264,87 @@
         <v>41275.537743055553</v>
       </c>
       <c r="G17" t="e">
-        <f t="shared" ref="G17:G51" si="12">1/0</f>
+        <f t="shared" ref="G17" si="14">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H17" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:8">
+      <c r="I17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.33434679572288706</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.4790641711458448E-2</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.15384324521947035</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.2839569177302782</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.71663331582968182</v>
+      </c>
+      <c r="N17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.1102236783988837</v>
+      </c>
+      <c r="O17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.55566680222390918</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.52373437529722899</v>
+      </c>
+      <c r="Q17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.18266820937029693</v>
+      </c>
+      <c r="R17">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.6129571602101413E-2</v>
+      </c>
+      <c r="S17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.91494941650842465</v>
+      </c>
+      <c r="T17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.7968682350225893</v>
+      </c>
+      <c r="U17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.22102540177556251</v>
+      </c>
+      <c r="V17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.84197389510203324</v>
+      </c>
+      <c r="W17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.19352690260319794</v>
+      </c>
+      <c r="X17">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.80993315378636688</v>
+      </c>
+      <c r="Y17">
+        <f t="shared" ref="Y17:Z51" ca="1" si="15">RAND()</f>
+        <v>0.4272421406586725</v>
+      </c>
+      <c r="Z17">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.23074436934685805</v>
+      </c>
+    </row>
+    <row r="18" spans="1:26">
       <c r="A18">
         <v>17</v>
       </c>
@@ -4101,15 +5361,87 @@
         <v>3.9351851851851852E-4</v>
       </c>
       <c r="G18" t="e">
-        <f t="shared" ref="G18:G51" si="13">something</f>
+        <f t="shared" ref="G18" si="16">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H18" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:8">
+      <c r="I18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.78127854754288317</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.72025037909441525</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.62004859107792343</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.84679739550041278</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.20920808682041714</v>
+      </c>
+      <c r="N18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.56707382713968646</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.12415910548864983</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.42414690741668071</v>
+      </c>
+      <c r="Q18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.85343775257205734</v>
+      </c>
+      <c r="R18">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.545248885487573E-2</v>
+      </c>
+      <c r="S18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.29905174165015425</v>
+      </c>
+      <c r="T18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.52382296482253166</v>
+      </c>
+      <c r="U18">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.4377138345431435E-2</v>
+      </c>
+      <c r="V18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.36657448120050673</v>
+      </c>
+      <c r="W18">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.4550500854841468E-2</v>
+      </c>
+      <c r="X18">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.858918846711484</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.11898286766032262</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.61003082156149924</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26">
       <c r="A19">
         <v>18</v>
       </c>
@@ -4126,15 +5458,87 @@
         <v>41277.156481481485</v>
       </c>
       <c r="G19" t="e">
-        <f t="shared" ref="G19:G51" si="14">"abc"+1</f>
+        <f t="shared" ref="G19" si="17">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H19" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
+      <c r="I19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.35851158412821316</v>
+      </c>
+      <c r="J19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.48687289963758973</v>
+      </c>
+      <c r="K19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.49933852630826381</v>
+      </c>
+      <c r="L19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.77966219902210165</v>
+      </c>
+      <c r="M19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.84020296380915738</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.14877138789911182</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.92676110767535014</v>
+      </c>
+      <c r="P19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.85293085130686452</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.87911394719680203</v>
+      </c>
+      <c r="R19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.73750354146374242</v>
+      </c>
+      <c r="S19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.43159484548096494</v>
+      </c>
+      <c r="T19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.49449667224311433</v>
+      </c>
+      <c r="U19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.60450348080146632</v>
+      </c>
+      <c r="V19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.2363856700905117</v>
+      </c>
+      <c r="W19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.83667353104492204</v>
+      </c>
+      <c r="X19">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.73733288542578612</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.45721542182466723</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.33618998514622866</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26">
       <c r="A20">
         <v>19</v>
       </c>
@@ -4151,15 +5555,87 @@
         <v>41278</v>
       </c>
       <c r="G20" t="e">
-        <f t="shared" ref="G20:G51" si="15">1/0</f>
+        <f t="shared" ref="G20" si="18">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H20" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:8">
+      <c r="I20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.34517904706005287</v>
+      </c>
+      <c r="J20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.93281461320923187</v>
+      </c>
+      <c r="K20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.21122236829485197</v>
+      </c>
+      <c r="L20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.42468305621702773</v>
+      </c>
+      <c r="M20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.31070135859004344</v>
+      </c>
+      <c r="N20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.2873853089177455</v>
+      </c>
+      <c r="O20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.6641334283485435</v>
+      </c>
+      <c r="P20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.14811721990154791</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.30041380770698134</v>
+      </c>
+      <c r="R20">
+        <f t="shared" ca="1" si="1"/>
+        <v>4.0241501111507372E-2</v>
+      </c>
+      <c r="S20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.38872424626458812</v>
+      </c>
+      <c r="T20">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.8290307180689505E-3</v>
+      </c>
+      <c r="U20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.5552989751495907</v>
+      </c>
+      <c r="V20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.45355744356569649</v>
+      </c>
+      <c r="W20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.38353042509830215</v>
+      </c>
+      <c r="X20">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.22899468010188873</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.68937591272370491</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" ca="1" si="15"/>
+        <v>4.1031650935316577E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26">
       <c r="A21">
         <v>20</v>
       </c>
@@ -4176,15 +5652,87 @@
         <v>41279.666666666664</v>
       </c>
       <c r="G21" t="e">
-        <f t="shared" ref="G21:G51" si="16">something</f>
+        <f t="shared" ref="G21" si="19">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H21" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:8">
+      <c r="I21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.51324216603869521</v>
+      </c>
+      <c r="J21">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.7779386113066442E-2</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.56098901562624048</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.97291836244183305</v>
+      </c>
+      <c r="M21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.62002585732344551</v>
+      </c>
+      <c r="N21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.7134832427734108</v>
+      </c>
+      <c r="O21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.79020970687498826</v>
+      </c>
+      <c r="P21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.80000344008958069</v>
+      </c>
+      <c r="Q21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.73933658917014344</v>
+      </c>
+      <c r="R21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.65386584379747315</v>
+      </c>
+      <c r="S21">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.6793876704100437E-2</v>
+      </c>
+      <c r="T21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.11425507253130263</v>
+      </c>
+      <c r="U21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.24784257238460905</v>
+      </c>
+      <c r="V21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.61136678938068278</v>
+      </c>
+      <c r="W21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.44119965974471997</v>
+      </c>
+      <c r="X21">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.87547026953962159</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.49317883835930643</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.42966940944120369</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26">
       <c r="A22">
         <v>21</v>
       </c>
@@ -4201,15 +5749,87 @@
         <v>41275.537743055553</v>
       </c>
       <c r="G22" t="e">
-        <f t="shared" ref="G22:G51" si="17">"abc"+1</f>
+        <f t="shared" ref="G22" si="20">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H22" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:8">
+      <c r="I22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.82577836840374352</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.46004174927559316</v>
+      </c>
+      <c r="K22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.44878332157665424</v>
+      </c>
+      <c r="L22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.84961404970991605</v>
+      </c>
+      <c r="M22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.91653167120873791</v>
+      </c>
+      <c r="N22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.58694612937396473</v>
+      </c>
+      <c r="O22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.96421802569841608</v>
+      </c>
+      <c r="P22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.59062967860469529</v>
+      </c>
+      <c r="Q22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.55453339438392879</v>
+      </c>
+      <c r="R22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.2540659914651151</v>
+      </c>
+      <c r="S22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.64609954777046974</v>
+      </c>
+      <c r="T22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.26525392615462873</v>
+      </c>
+      <c r="U22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.47676116932729329</v>
+      </c>
+      <c r="V22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.33075791969616319</v>
+      </c>
+      <c r="W22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.87040550462359534</v>
+      </c>
+      <c r="X22">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.73941578469477887</v>
+      </c>
+      <c r="Y22">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.28198578969169608</v>
+      </c>
+      <c r="Z22">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.45727955999708569</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26">
       <c r="A23">
         <v>22</v>
       </c>
@@ -4226,15 +5846,87 @@
         <v>3.9351851851851852E-4</v>
       </c>
       <c r="G23" t="e">
-        <f t="shared" ref="G23:G51" si="18">1/0</f>
+        <f t="shared" ref="G23" si="21">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H23" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:8">
+      <c r="I23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.30261518276344435</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.17272329472992265</v>
+      </c>
+      <c r="K23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.21948874491024684</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.75768823296481269</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.78010720381133147</v>
+      </c>
+      <c r="N23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.25431962539427888</v>
+      </c>
+      <c r="O23">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.5093396581618834E-2</v>
+      </c>
+      <c r="P23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.10632722845624254</v>
+      </c>
+      <c r="Q23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.28334160672417419</v>
+      </c>
+      <c r="R23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.47417839261518502</v>
+      </c>
+      <c r="S23">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.3365173255803331E-2</v>
+      </c>
+      <c r="T23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.31245401877481438</v>
+      </c>
+      <c r="U23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9758260549142983</v>
+      </c>
+      <c r="V23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.3963644434426139</v>
+      </c>
+      <c r="W23">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.13139765206923881</v>
+      </c>
+      <c r="X23">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.052810240717351E-2</v>
+      </c>
+      <c r="Y23">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.23586239588717339</v>
+      </c>
+      <c r="Z23">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.54636810294328764</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26">
       <c r="A24">
         <v>23</v>
       </c>
@@ -4251,15 +5943,87 @@
         <v>41277.156481481485</v>
       </c>
       <c r="G24" t="e">
-        <f t="shared" ref="G24:G51" si="19">something</f>
+        <f t="shared" ref="G24" si="22">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H24" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:8">
+      <c r="I24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.13960986487165283</v>
+      </c>
+      <c r="J24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.7374867318435997</v>
+      </c>
+      <c r="K24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.28175071052472056</v>
+      </c>
+      <c r="L24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.11322738040928082</v>
+      </c>
+      <c r="M24">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.7036837018786164E-2</v>
+      </c>
+      <c r="N24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.87308436244938303</v>
+      </c>
+      <c r="O24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.71718153187536005</v>
+      </c>
+      <c r="P24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.84681498950210266</v>
+      </c>
+      <c r="Q24">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.1494550607613618E-2</v>
+      </c>
+      <c r="R24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.32935651182763237</v>
+      </c>
+      <c r="S24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.4247779481037447</v>
+      </c>
+      <c r="T24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.99556036490739674</v>
+      </c>
+      <c r="U24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.45001719721813105</v>
+      </c>
+      <c r="V24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.51549465652892279</v>
+      </c>
+      <c r="W24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.64131433794717208</v>
+      </c>
+      <c r="X24">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.17892342720336807</v>
+      </c>
+      <c r="Y24">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.74113020118078521</v>
+      </c>
+      <c r="Z24">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.52704941135523464</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26">
       <c r="A25">
         <v>24</v>
       </c>
@@ -4276,15 +6040,87 @@
         <v>41278</v>
       </c>
       <c r="G25" t="e">
-        <f t="shared" ref="G25:G51" si="20">"abc"+1</f>
+        <f t="shared" ref="G25" si="23">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H25" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:8">
+      <c r="I25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.32091772162757815</v>
+      </c>
+      <c r="J25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.88312148507865373</v>
+      </c>
+      <c r="K25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.98832286736135366</v>
+      </c>
+      <c r="L25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.65238221109716787</v>
+      </c>
+      <c r="M25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.29238196770688241</v>
+      </c>
+      <c r="N25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.1618456156836221</v>
+      </c>
+      <c r="O25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.36541780299891269</v>
+      </c>
+      <c r="P25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.58857626505082261</v>
+      </c>
+      <c r="Q25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.56584297981395093</v>
+      </c>
+      <c r="R25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.16102729460177623</v>
+      </c>
+      <c r="S25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.28831510361668233</v>
+      </c>
+      <c r="T25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.64777867417405433</v>
+      </c>
+      <c r="U25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.80587690235168175</v>
+      </c>
+      <c r="V25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.5674592504623206</v>
+      </c>
+      <c r="W25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.87199802766897427</v>
+      </c>
+      <c r="X25">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.57914908849274305</v>
+      </c>
+      <c r="Y25">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.4297795006107874</v>
+      </c>
+      <c r="Z25">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.78297353275075554</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26">
       <c r="A26">
         <v>25</v>
       </c>
@@ -4301,15 +6137,87 @@
         <v>41279.666666666664</v>
       </c>
       <c r="G26" t="e">
-        <f t="shared" ref="G26:G51" si="21">1/0</f>
+        <f t="shared" ref="G26" si="24">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H26" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:8">
+      <c r="I26">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.25174773609812706</v>
+      </c>
+      <c r="J26">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.46257217512822491</v>
+      </c>
+      <c r="K26">
+        <f t="shared" ca="1" si="1"/>
+        <v>5.6981014256934581E-2</v>
+      </c>
+      <c r="L26">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.88991707337697235</v>
+      </c>
+      <c r="M26">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.62448711260798406</v>
+      </c>
+      <c r="N26">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.37388616435466859</v>
+      </c>
+      <c r="O26">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.8862922505031956</v>
+      </c>
+      <c r="P26">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.37391738743759628</v>
+      </c>
+      <c r="Q26">
+        <f t="shared" ca="1" si="1"/>
+        <v>3.969316534721723E-2</v>
+      </c>
+      <c r="R26">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.3944090362624183</v>
+      </c>
+      <c r="S26">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.78902051444845545</v>
+      </c>
+      <c r="T26">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.70504330232703494</v>
+      </c>
+      <c r="U26">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.72257847683491361</v>
+      </c>
+      <c r="V26">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.2097684791554206E-2</v>
+      </c>
+      <c r="W26">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.7026877365739654E-2</v>
+      </c>
+      <c r="X26">
+        <f t="shared" ca="1" si="1"/>
+        <v>2.290882703782815E-2</v>
+      </c>
+      <c r="Y26">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.56165823710078355</v>
+      </c>
+      <c r="Z26">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.37868614168484638</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26">
       <c r="A27">
         <v>26</v>
       </c>
@@ -4326,15 +6234,87 @@
         <v>41275.537743055553</v>
       </c>
       <c r="G27" t="e">
-        <f t="shared" ref="G27:G51" si="22">something</f>
+        <f t="shared" ref="G27" si="25">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H27" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:8">
+      <c r="I27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.84459778292634724</v>
+      </c>
+      <c r="J27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.43810862973409481</v>
+      </c>
+      <c r="K27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.68104437244205229</v>
+      </c>
+      <c r="L27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.25541604291652742</v>
+      </c>
+      <c r="M27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.98369197873083969</v>
+      </c>
+      <c r="N27">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.0052484881735935E-2</v>
+      </c>
+      <c r="O27">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.7488526166453195E-2</v>
+      </c>
+      <c r="P27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.60738909000247998</v>
+      </c>
+      <c r="Q27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.1568160766698572</v>
+      </c>
+      <c r="R27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.92885817853873498</v>
+      </c>
+      <c r="S27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.32305190661518313</v>
+      </c>
+      <c r="T27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.91109971001734846</v>
+      </c>
+      <c r="U27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.89055265212363932</v>
+      </c>
+      <c r="V27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.28256801459674075</v>
+      </c>
+      <c r="W27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.17340849166097938</v>
+      </c>
+      <c r="X27">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.36833222352055173</v>
+      </c>
+      <c r="Y27">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.56469326694351984</v>
+      </c>
+      <c r="Z27">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.18802851836982615</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26">
       <c r="A28">
         <v>27</v>
       </c>
@@ -4351,15 +6331,87 @@
         <v>3.9351851851851852E-4</v>
       </c>
       <c r="G28" t="e">
-        <f t="shared" ref="G28:G51" si="23">"abc"+1</f>
+        <f t="shared" ref="G28" si="26">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H28" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:8">
+      <c r="I28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.98502600326201939</v>
+      </c>
+      <c r="J28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.24933994210080179</v>
+      </c>
+      <c r="K28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.63222437052010161</v>
+      </c>
+      <c r="L28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.11354711221471658</v>
+      </c>
+      <c r="M28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.85169619067209001</v>
+      </c>
+      <c r="N28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.41439015951675728</v>
+      </c>
+      <c r="O28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.14808430615101409</v>
+      </c>
+      <c r="P28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.87736014842378007</v>
+      </c>
+      <c r="Q28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.95209094140141226</v>
+      </c>
+      <c r="R28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.16486243285546442</v>
+      </c>
+      <c r="S28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.13583670267770886</v>
+      </c>
+      <c r="T28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.2351040834957393</v>
+      </c>
+      <c r="U28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.58285332105187271</v>
+      </c>
+      <c r="V28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.15367149835535943</v>
+      </c>
+      <c r="W28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.42860476090249311</v>
+      </c>
+      <c r="X28">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.19427560151728929</v>
+      </c>
+      <c r="Y28">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.19126660309941235</v>
+      </c>
+      <c r="Z28">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.97449501704281594</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26">
       <c r="A29">
         <v>28</v>
       </c>
@@ -4376,15 +6428,87 @@
         <v>41277.156481481485</v>
       </c>
       <c r="G29" t="e">
-        <f t="shared" ref="G29:G51" si="24">1/0</f>
+        <f t="shared" ref="G29" si="27">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H29" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:8">
+      <c r="I29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.52850264894880594</v>
+      </c>
+      <c r="J29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.53597969092571651</v>
+      </c>
+      <c r="K29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.52121530630716573</v>
+      </c>
+      <c r="L29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9038501696069241</v>
+      </c>
+      <c r="M29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.63468634627809517</v>
+      </c>
+      <c r="N29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.62404931895922988</v>
+      </c>
+      <c r="O29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.44941764687864083</v>
+      </c>
+      <c r="P29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.48841127013817898</v>
+      </c>
+      <c r="Q29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.36044669758176529</v>
+      </c>
+      <c r="R29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.14460938616746266</v>
+      </c>
+      <c r="S29">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.0988472350892784E-2</v>
+      </c>
+      <c r="T29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.67091314704033911</v>
+      </c>
+      <c r="U29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.47724409789434741</v>
+      </c>
+      <c r="V29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.83524895451805981</v>
+      </c>
+      <c r="W29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.83432298659317172</v>
+      </c>
+      <c r="X29">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.41552993982584685</v>
+      </c>
+      <c r="Y29">
+        <f t="shared" ca="1" si="15"/>
+        <v>1.445660753415523E-2</v>
+      </c>
+      <c r="Z29">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.44387311149138986</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26">
       <c r="A30">
         <v>29</v>
       </c>
@@ -4401,15 +6525,87 @@
         <v>41278</v>
       </c>
       <c r="G30" t="e">
-        <f t="shared" ref="G30:G51" si="25">something</f>
+        <f t="shared" ref="G30" si="28">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H30" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:8">
+      <c r="I30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.69903099502386368</v>
+      </c>
+      <c r="J30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.95501456358266734</v>
+      </c>
+      <c r="K30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.69333855995245053</v>
+      </c>
+      <c r="L30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.77800884398334647</v>
+      </c>
+      <c r="M30">
+        <f t="shared" ca="1" si="1"/>
+        <v>1.6238553011229673E-3</v>
+      </c>
+      <c r="N30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.96813633102737373</v>
+      </c>
+      <c r="O30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.58997308520711889</v>
+      </c>
+      <c r="P30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.38247313579926767</v>
+      </c>
+      <c r="Q30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.52663831206468192</v>
+      </c>
+      <c r="R30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.90681770161188413</v>
+      </c>
+      <c r="S30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.73518649999962726</v>
+      </c>
+      <c r="T30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.31881695647749764</v>
+      </c>
+      <c r="U30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.40711165104133196</v>
+      </c>
+      <c r="V30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.70950245954213265</v>
+      </c>
+      <c r="W30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.48980218511500195</v>
+      </c>
+      <c r="X30">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.80650888710547064</v>
+      </c>
+      <c r="Y30">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.25569783090060438</v>
+      </c>
+      <c r="Z30">
+        <f t="shared" ca="1" si="15"/>
+        <v>3.0604810810463956E-3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:26">
       <c r="A31">
         <v>30</v>
       </c>
@@ -4426,15 +6622,87 @@
         <v>41279.666666666664</v>
       </c>
       <c r="G31" t="e">
-        <f t="shared" ref="G31:G51" si="26">"abc"+1</f>
+        <f t="shared" ref="G31" si="29">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H31" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:8">
+      <c r="I31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.9309685241163812</v>
+      </c>
+      <c r="J31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.26147568721473147</v>
+      </c>
+      <c r="K31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.26488730752605427</v>
+      </c>
+      <c r="L31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.28728254868391945</v>
+      </c>
+      <c r="M31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.5028804263372888</v>
+      </c>
+      <c r="N31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.77782942061124805</v>
+      </c>
+      <c r="O31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.22590594646583539</v>
+      </c>
+      <c r="P31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.38877325920610806</v>
+      </c>
+      <c r="Q31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.19415065097549034</v>
+      </c>
+      <c r="R31">
+        <f t="shared" ca="1" si="1"/>
+        <v>7.8485978753456975E-2</v>
+      </c>
+      <c r="S31">
+        <f t="shared" ca="1" si="1"/>
+        <v>8.5310670789624732E-2</v>
+      </c>
+      <c r="T31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.64093496944399364</v>
+      </c>
+      <c r="U31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.33864082721203226</v>
+      </c>
+      <c r="V31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.10894798927992611</v>
+      </c>
+      <c r="W31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.45536931555193338</v>
+      </c>
+      <c r="X31">
+        <f t="shared" ca="1" si="1"/>
+        <v>0.34305458536777211</v>
+      </c>
+      <c r="Y31">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.12517574617158922</v>
+      </c>
+      <c r="Z31">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.5462747773319796</v>
+      </c>
+    </row>
+    <row r="32" spans="1:26">
       <c r="A32">
         <v>31</v>
       </c>
@@ -4451,15 +6719,87 @@
         <v>41275.537743055553</v>
       </c>
       <c r="G32" t="e">
-        <f t="shared" ref="G32:G51" si="27">1/0</f>
+        <f t="shared" ref="G32" si="30">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H32" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:8">
+      <c r="I32">
+        <f t="shared" ca="1" si="1"/>
+        <v>6.9553828795635875E-2</v>
+      </c>
+      <c r="J32">
+        <f t="shared" ref="J32:Y51" ca="1" si="31">RAND()</f>
+        <v>0.53489350264938818</v>
+      </c>
+      <c r="K32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.33741040834600422</v>
+      </c>
+      <c r="L32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.88239322092352268</v>
+      </c>
+      <c r="M32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.64498010191809751</v>
+      </c>
+      <c r="N32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.94202595807591394</v>
+      </c>
+      <c r="O32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.39235960766118294</v>
+      </c>
+      <c r="P32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.99725761382433575</v>
+      </c>
+      <c r="Q32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.31272493257599798</v>
+      </c>
+      <c r="R32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.64297130159782045</v>
+      </c>
+      <c r="S32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.82764003884789139</v>
+      </c>
+      <c r="T32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.73389559362952761</v>
+      </c>
+      <c r="U32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.34291500838660249</v>
+      </c>
+      <c r="V32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.18973445717918014</v>
+      </c>
+      <c r="W32">
+        <f t="shared" ca="1" si="31"/>
+        <v>4.5885780578128199E-2</v>
+      </c>
+      <c r="X32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.31292250443137681</v>
+      </c>
+      <c r="Y32">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.83141685044133296</v>
+      </c>
+      <c r="Z32">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.53028967965483065</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4476,15 +6816,87 @@
         <v>3.9351851851851852E-4</v>
       </c>
       <c r="G33" t="e">
-        <f t="shared" ref="G33:G51" si="28">something</f>
+        <f t="shared" ref="G33" si="32">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H33" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:8">
+      <c r="I33">
+        <f t="shared" ref="I33:X51" ca="1" si="33">RAND()</f>
+        <v>0.88019749957049787</v>
+      </c>
+      <c r="J33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.25563975052911181</v>
+      </c>
+      <c r="K33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.93970067788843659</v>
+      </c>
+      <c r="L33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.62815273773103764</v>
+      </c>
+      <c r="M33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.35435460438781197</v>
+      </c>
+      <c r="N33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.37754565603111145</v>
+      </c>
+      <c r="O33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.61919441131534991</v>
+      </c>
+      <c r="P33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.96306152021850133</v>
+      </c>
+      <c r="Q33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.48319862586495976</v>
+      </c>
+      <c r="R33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.17734634898608637</v>
+      </c>
+      <c r="S33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.91914432090012321</v>
+      </c>
+      <c r="T33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.96847836703759393</v>
+      </c>
+      <c r="U33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.1448553598331761</v>
+      </c>
+      <c r="V33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.17776199255992242</v>
+      </c>
+      <c r="W33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.46457604349377235</v>
+      </c>
+      <c r="X33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.52920978136045782</v>
+      </c>
+      <c r="Y33">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.88856171589749899</v>
+      </c>
+      <c r="Z33">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.8266649872410422</v>
+      </c>
+    </row>
+    <row r="34" spans="1:26">
       <c r="A34">
         <v>33</v>
       </c>
@@ -4501,15 +6913,87 @@
         <v>41277.156481481485</v>
       </c>
       <c r="G34" t="e">
-        <f t="shared" ref="G34:G51" si="29">"abc"+1</f>
+        <f t="shared" ref="G34" si="34">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H34" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:8">
+      <c r="I34">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.81719794370577847</v>
+      </c>
+      <c r="J34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.94919405638182652</v>
+      </c>
+      <c r="K34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.24365461529554366</v>
+      </c>
+      <c r="L34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.40843020491562176</v>
+      </c>
+      <c r="M34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.39061983716977566</v>
+      </c>
+      <c r="N34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.47459263312337796</v>
+      </c>
+      <c r="O34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.93164531959927266</v>
+      </c>
+      <c r="P34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.14752287564191269</v>
+      </c>
+      <c r="Q34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.56536681516255172</v>
+      </c>
+      <c r="R34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.21849589012311965</v>
+      </c>
+      <c r="S34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.11997723725436182</v>
+      </c>
+      <c r="T34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.26936145168421244</v>
+      </c>
+      <c r="U34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.16654752949987239</v>
+      </c>
+      <c r="V34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.38189525988478423</v>
+      </c>
+      <c r="W34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.7926119605635833</v>
+      </c>
+      <c r="X34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.37851605522238518</v>
+      </c>
+      <c r="Y34">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.95775157529061516</v>
+      </c>
+      <c r="Z34">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.55861579688149232</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26">
       <c r="A35">
         <v>34</v>
       </c>
@@ -4526,15 +7010,87 @@
         <v>41278</v>
       </c>
       <c r="G35" t="e">
-        <f t="shared" ref="G35:G51" si="30">1/0</f>
+        <f t="shared" ref="G35" si="35">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H35" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="36" spans="1:8">
+      <c r="I35">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.45395863281056315</v>
+      </c>
+      <c r="J35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.88061057925538544</v>
+      </c>
+      <c r="K35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.92159984333828115</v>
+      </c>
+      <c r="L35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.6392544480654152</v>
+      </c>
+      <c r="M35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.31180269710765285</v>
+      </c>
+      <c r="N35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.7297982714732657</v>
+      </c>
+      <c r="O35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.18005187408909973</v>
+      </c>
+      <c r="P35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.85740635088377481</v>
+      </c>
+      <c r="Q35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.32316539603996297</v>
+      </c>
+      <c r="R35">
+        <f t="shared" ca="1" si="31"/>
+        <v>4.4339802503530756E-2</v>
+      </c>
+      <c r="S35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.18685042382581263</v>
+      </c>
+      <c r="T35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.53841309287575045</v>
+      </c>
+      <c r="U35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.74687634316128071</v>
+      </c>
+      <c r="V35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.63068195174579755</v>
+      </c>
+      <c r="W35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.23125378944334152</v>
+      </c>
+      <c r="X35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.53220463013527386</v>
+      </c>
+      <c r="Y35">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.64559310872856457</v>
+      </c>
+      <c r="Z35">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.21981240460020601</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26">
       <c r="A36">
         <v>35</v>
       </c>
@@ -4551,15 +7107,87 @@
         <v>41279.666666666664</v>
       </c>
       <c r="G36" t="e">
-        <f t="shared" ref="G36:G51" si="31">something</f>
+        <f t="shared" ref="G36" si="36">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H36" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:8">
+      <c r="I36">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.75287264608156057</v>
+      </c>
+      <c r="J36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.13627792787538073</v>
+      </c>
+      <c r="K36">
+        <f t="shared" ca="1" si="31"/>
+        <v>9.4347038979424536E-2</v>
+      </c>
+      <c r="L36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.23257088422271111</v>
+      </c>
+      <c r="M36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.48436435214161788</v>
+      </c>
+      <c r="N36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.8402682273917399</v>
+      </c>
+      <c r="O36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.69303099878404584</v>
+      </c>
+      <c r="P36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.82290435873405132</v>
+      </c>
+      <c r="Q36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.14070982294808287</v>
+      </c>
+      <c r="R36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.38189681299896727</v>
+      </c>
+      <c r="S36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.60655415779773492</v>
+      </c>
+      <c r="T36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.39249122306973661</v>
+      </c>
+      <c r="U36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.75395819708018086</v>
+      </c>
+      <c r="V36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.27528552372215209</v>
+      </c>
+      <c r="W36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.49688934304637322</v>
+      </c>
+      <c r="X36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.38732590880080398</v>
+      </c>
+      <c r="Y36">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.65075591884766204</v>
+      </c>
+      <c r="Z36">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.31396727427076598</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26">
       <c r="A37">
         <v>36</v>
       </c>
@@ -4576,15 +7204,87 @@
         <v>41275.537743055553</v>
       </c>
       <c r="G37" t="e">
-        <f t="shared" ref="G37:G51" si="32">"abc"+1</f>
+        <f t="shared" ref="G37" si="37">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H37" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:8">
+      <c r="I37">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.1120524566556037</v>
+      </c>
+      <c r="J37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.97872568096959633</v>
+      </c>
+      <c r="K37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.30800547143318335</v>
+      </c>
+      <c r="L37">
+        <f t="shared" ca="1" si="31"/>
+        <v>3.9504749110852E-2</v>
+      </c>
+      <c r="M37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.44401974924335041</v>
+      </c>
+      <c r="N37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.19485813539878916</v>
+      </c>
+      <c r="O37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.12194084600736832</v>
+      </c>
+      <c r="P37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.86555154430134063</v>
+      </c>
+      <c r="Q37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.64883308298851916</v>
+      </c>
+      <c r="R37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.38654209893031932</v>
+      </c>
+      <c r="S37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.2230900578500421</v>
+      </c>
+      <c r="T37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.38136302359321528</v>
+      </c>
+      <c r="U37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.48704122815809414</v>
+      </c>
+      <c r="V37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.64017953869154887</v>
+      </c>
+      <c r="W37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.8209953585866242</v>
+      </c>
+      <c r="X37">
+        <f t="shared" ca="1" si="31"/>
+        <v>3.030867113704705E-3</v>
+      </c>
+      <c r="Y37">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.68867020145705571</v>
+      </c>
+      <c r="Z37">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.41888971410392339</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26">
       <c r="A38">
         <v>37</v>
       </c>
@@ -4601,15 +7301,87 @@
         <v>3.9351851851851852E-4</v>
       </c>
       <c r="G38" t="e">
-        <f t="shared" ref="G38:G51" si="33">1/0</f>
+        <f t="shared" ref="G38" si="38">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H38" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:8">
+      <c r="I38">
+        <f t="shared" ca="1" si="33"/>
+        <v>1.8247714478433763E-2</v>
+      </c>
+      <c r="J38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.29204785569050629</v>
+      </c>
+      <c r="K38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.67627581644723078</v>
+      </c>
+      <c r="L38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.92950945136462992</v>
+      </c>
+      <c r="M38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.25313370990037942</v>
+      </c>
+      <c r="N38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.94971711216058496</v>
+      </c>
+      <c r="O38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.86553557395304093</v>
+      </c>
+      <c r="P38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.2425993500430953</v>
+      </c>
+      <c r="Q38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.71072212303920168</v>
+      </c>
+      <c r="R38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.33624063012991423</v>
+      </c>
+      <c r="S38">
+        <f t="shared" ca="1" si="31"/>
+        <v>7.1111612388893741E-2</v>
+      </c>
+      <c r="T38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.72325708824497492</v>
+      </c>
+      <c r="U38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.20029105643557699</v>
+      </c>
+      <c r="V38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.14872156671663261</v>
+      </c>
+      <c r="W38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.43679757314452428</v>
+      </c>
+      <c r="X38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.984723427436483</v>
+      </c>
+      <c r="Y38">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.39226064484313217</v>
+      </c>
+      <c r="Z38">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.77515566902652022</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26">
       <c r="A39">
         <v>38</v>
       </c>
@@ -4626,15 +7398,87 @@
         <v>41277.156481481485</v>
       </c>
       <c r="G39" t="e">
-        <f t="shared" ref="G39:G51" si="34">something</f>
+        <f t="shared" ref="G39" si="39">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H39" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:8">
+      <c r="I39">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.21370705948623181</v>
+      </c>
+      <c r="J39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.54799988310342307</v>
+      </c>
+      <c r="K39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.57987441655886274</v>
+      </c>
+      <c r="L39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.72080783409947802</v>
+      </c>
+      <c r="M39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.72015100118167974</v>
+      </c>
+      <c r="N39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.82069090302888437</v>
+      </c>
+      <c r="O39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.53683016061585964</v>
+      </c>
+      <c r="P39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.59212484192886061</v>
+      </c>
+      <c r="Q39">
+        <f t="shared" ca="1" si="31"/>
+        <v>8.8347254041373113E-2</v>
+      </c>
+      <c r="R39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.49658859738342576</v>
+      </c>
+      <c r="S39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.59593939277291597</v>
+      </c>
+      <c r="T39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.36205012336859854</v>
+      </c>
+      <c r="U39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.40109541553379058</v>
+      </c>
+      <c r="V39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.55889686692608676</v>
+      </c>
+      <c r="W39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.79290095283038753</v>
+      </c>
+      <c r="X39">
+        <f t="shared" ca="1" si="31"/>
+        <v>7.9667853546275702E-2</v>
+      </c>
+      <c r="Y39">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.13161964797125247</v>
+      </c>
+      <c r="Z39">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.13447175180449411</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4651,15 +7495,87 @@
         <v>41278</v>
       </c>
       <c r="G40" t="e">
-        <f t="shared" ref="G40:G51" si="35">"abc"+1</f>
+        <f t="shared" ref="G40" si="40">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H40" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="41" spans="1:8">
+      <c r="I40">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.80659205183779037</v>
+      </c>
+      <c r="J40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.45576442975191056</v>
+      </c>
+      <c r="K40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.37900192447047554</v>
+      </c>
+      <c r="L40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.12938833719682141</v>
+      </c>
+      <c r="M40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.49585000591790129</v>
+      </c>
+      <c r="N40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.58449456891258178</v>
+      </c>
+      <c r="O40">
+        <f t="shared" ca="1" si="31"/>
+        <v>9.2402950232197467E-2</v>
+      </c>
+      <c r="P40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.89203931747047849</v>
+      </c>
+      <c r="Q40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.24071351244620254</v>
+      </c>
+      <c r="R40">
+        <f t="shared" ca="1" si="31"/>
+        <v>2.7547395454566304E-2</v>
+      </c>
+      <c r="S40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.40470775933834724</v>
+      </c>
+      <c r="T40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.72653181400242228</v>
+      </c>
+      <c r="U40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.66987567213400523</v>
+      </c>
+      <c r="V40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.62171282314689014</v>
+      </c>
+      <c r="W40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.76869337466757803</v>
+      </c>
+      <c r="X40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.27750809539375054</v>
+      </c>
+      <c r="Y40">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.77540377453821718</v>
+      </c>
+      <c r="Z40">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.11456372883623422</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4676,15 +7592,87 @@
         <v>41279.666666666664</v>
       </c>
       <c r="G41" t="e">
-        <f t="shared" ref="G41:G51" si="36">1/0</f>
+        <f t="shared" ref="G41" si="41">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H41" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:8">
+      <c r="I41">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.30049027944513185</v>
+      </c>
+      <c r="J41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.53998289492050733</v>
+      </c>
+      <c r="K41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.91284376397895672</v>
+      </c>
+      <c r="L41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.66488326061160097</v>
+      </c>
+      <c r="M41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.57006397976992385</v>
+      </c>
+      <c r="N41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.32995461284273442</v>
+      </c>
+      <c r="O41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.75340791255040718</v>
+      </c>
+      <c r="P41">
+        <f t="shared" ca="1" si="31"/>
+        <v>3.8071533694683635E-2</v>
+      </c>
+      <c r="Q41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.67921013284906062</v>
+      </c>
+      <c r="R41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.39328319802766942</v>
+      </c>
+      <c r="S41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.7236759763342635</v>
+      </c>
+      <c r="T41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.58555744897493223</v>
+      </c>
+      <c r="U41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.246873445087611</v>
+      </c>
+      <c r="V41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.50738438140270448</v>
+      </c>
+      <c r="W41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.94162024429517754</v>
+      </c>
+      <c r="X41">
+        <f t="shared" ca="1" si="31"/>
+        <v>1.6089715404404514E-2</v>
+      </c>
+      <c r="Y41">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.39175039908391884</v>
+      </c>
+      <c r="Z41">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.98537222843218686</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4701,15 +7689,87 @@
         <v>41275.537743055553</v>
       </c>
       <c r="G42" t="e">
-        <f t="shared" ref="G42:G51" si="37">something</f>
+        <f t="shared" ref="G42" si="42">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H42" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:8">
+      <c r="I42">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.74281473521184793</v>
+      </c>
+      <c r="J42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.81256770081802232</v>
+      </c>
+      <c r="K42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.74427856712640628</v>
+      </c>
+      <c r="L42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.50736729868699126</v>
+      </c>
+      <c r="M42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.34019293162226316</v>
+      </c>
+      <c r="N42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.66165442311301492</v>
+      </c>
+      <c r="O42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.79661093348252776</v>
+      </c>
+      <c r="P42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.13190244953506647</v>
+      </c>
+      <c r="Q42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.11383127659267034</v>
+      </c>
+      <c r="R42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.85444322769477921</v>
+      </c>
+      <c r="S42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.44605455937395333</v>
+      </c>
+      <c r="T42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.83041920418871895</v>
+      </c>
+      <c r="U42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.94859919830616879</v>
+      </c>
+      <c r="V42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.76151623454151895</v>
+      </c>
+      <c r="W42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.85276861415676031</v>
+      </c>
+      <c r="X42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.10014156366645766</v>
+      </c>
+      <c r="Y42">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.59114373591984704</v>
+      </c>
+      <c r="Z42">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.48524998165888411</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4726,15 +7786,87 @@
         <v>3.9351851851851852E-4</v>
       </c>
       <c r="G43" t="e">
-        <f t="shared" ref="G43:G51" si="38">"abc"+1</f>
+        <f t="shared" ref="G43" si="43">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H43" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:8">
+      <c r="I43">
+        <f t="shared" ca="1" si="33"/>
+        <v>5.6698666762759142E-2</v>
+      </c>
+      <c r="J43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.86605866082487626</v>
+      </c>
+      <c r="K43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.13877772243479958</v>
+      </c>
+      <c r="L43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.35077644083891624</v>
+      </c>
+      <c r="M43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.83534363565702674</v>
+      </c>
+      <c r="N43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.8604726515841119</v>
+      </c>
+      <c r="O43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.92475527139417402</v>
+      </c>
+      <c r="P43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.2308208029968366</v>
+      </c>
+      <c r="Q43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.91256999990494969</v>
+      </c>
+      <c r="R43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.58798236855383135</v>
+      </c>
+      <c r="S43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.57350906083565101</v>
+      </c>
+      <c r="T43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.16553443147810831</v>
+      </c>
+      <c r="U43">
+        <f t="shared" ca="1" si="31"/>
+        <v>6.810956583075356E-2</v>
+      </c>
+      <c r="V43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.42720438520997051</v>
+      </c>
+      <c r="W43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.55580983513300986</v>
+      </c>
+      <c r="X43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.31347602220981174</v>
+      </c>
+      <c r="Y43">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.80557552969689461</v>
+      </c>
+      <c r="Z43">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.74517069028599958</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4751,15 +7883,87 @@
         <v>41277.156481481485</v>
       </c>
       <c r="G44" t="e">
-        <f t="shared" ref="G44:G51" si="39">1/0</f>
+        <f t="shared" ref="G44" si="44">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H44" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="45" spans="1:8">
+      <c r="I44">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.68576661136476424</v>
+      </c>
+      <c r="J44">
+        <f t="shared" ca="1" si="31"/>
+        <v>6.837187856981386E-2</v>
+      </c>
+      <c r="K44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.60004094636768335</v>
+      </c>
+      <c r="L44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.81985329075694213</v>
+      </c>
+      <c r="M44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.57659009213849621</v>
+      </c>
+      <c r="N44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.5263607132746867</v>
+      </c>
+      <c r="O44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.68327473442696252</v>
+      </c>
+      <c r="P44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.1872495228662906</v>
+      </c>
+      <c r="Q44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.94305115992701427</v>
+      </c>
+      <c r="R44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.20829824750445924</v>
+      </c>
+      <c r="S44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.38518352950761747</v>
+      </c>
+      <c r="T44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.7876654944865813</v>
+      </c>
+      <c r="U44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.69788065283440082</v>
+      </c>
+      <c r="V44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.39016660606038478</v>
+      </c>
+      <c r="W44">
+        <f t="shared" ca="1" si="31"/>
+        <v>1.9048398793540033E-2</v>
+      </c>
+      <c r="X44">
+        <f t="shared" ca="1" si="31"/>
+        <v>3.2479334592128484E-2</v>
+      </c>
+      <c r="Y44">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.43449691229788923</v>
+      </c>
+      <c r="Z44">
+        <f t="shared" ca="1" si="15"/>
+        <v>6.0883995440703331E-2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4776,15 +7980,87 @@
         <v>41278</v>
       </c>
       <c r="G45" t="e">
-        <f t="shared" ref="G45:G51" si="40">something</f>
+        <f t="shared" ref="G45" si="45">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H45" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="46" spans="1:8">
+      <c r="I45">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.41363116384732168</v>
+      </c>
+      <c r="J45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.89349892809183462</v>
+      </c>
+      <c r="K45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.56880808328960475</v>
+      </c>
+      <c r="L45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.41799741562671389</v>
+      </c>
+      <c r="M45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.9514745170329002</v>
+      </c>
+      <c r="N45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.39141368782429675</v>
+      </c>
+      <c r="O45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.59335720698765848</v>
+      </c>
+      <c r="P45">
+        <f t="shared" ca="1" si="31"/>
+        <v>9.3846386364227152E-2</v>
+      </c>
+      <c r="Q45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.43687201664901831</v>
+      </c>
+      <c r="R45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.44371390549454071</v>
+      </c>
+      <c r="S45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.57458125743280208</v>
+      </c>
+      <c r="T45">
+        <f t="shared" ca="1" si="31"/>
+        <v>5.4055527228222933E-2</v>
+      </c>
+      <c r="U45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.65755185758920476</v>
+      </c>
+      <c r="V45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.94566175547383136</v>
+      </c>
+      <c r="W45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.77293258608907567</v>
+      </c>
+      <c r="X45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.2037066383934788</v>
+      </c>
+      <c r="Y45">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.10396786355417331</v>
+      </c>
+      <c r="Z45">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.78859377985688783</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26">
       <c r="A46">
         <v>45</v>
       </c>
@@ -4801,15 +8077,87 @@
         <v>41279.666666666664</v>
       </c>
       <c r="G46" t="e">
-        <f t="shared" ref="G46:G51" si="41">"abc"+1</f>
+        <f t="shared" ref="G46" si="46">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H46" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="47" spans="1:8">
+      <c r="I46">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.78419948264729733</v>
+      </c>
+      <c r="J46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.48418214562355999</v>
+      </c>
+      <c r="K46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.18893820265345207</v>
+      </c>
+      <c r="L46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.77010432737112722</v>
+      </c>
+      <c r="M46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.48706772579621338</v>
+      </c>
+      <c r="N46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.96171181619454471</v>
+      </c>
+      <c r="O46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.53677185081692524</v>
+      </c>
+      <c r="P46">
+        <f t="shared" ca="1" si="31"/>
+        <v>4.1769844699178327E-2</v>
+      </c>
+      <c r="Q46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.45848089522654678</v>
+      </c>
+      <c r="R46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.58767079342473072</v>
+      </c>
+      <c r="S46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.56265196836344389</v>
+      </c>
+      <c r="T46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.49947249144810002</v>
+      </c>
+      <c r="U46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.2952317271557785</v>
+      </c>
+      <c r="V46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.23714254208176089</v>
+      </c>
+      <c r="W46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.92087153471270744</v>
+      </c>
+      <c r="X46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.95863299594980722</v>
+      </c>
+      <c r="Y46">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.35162250322327049</v>
+      </c>
+      <c r="Z46">
+        <f t="shared" ca="1" si="15"/>
+        <v>0.64685285418701521</v>
+      </c>
+    </row>
+    <row r="47" spans="1:26">
       <c r="A47">
         <v>46</v>
       </c>
@@ -4826,15 +8174,87 @@
         <v>41275.537743055553</v>
       </c>
       <c r="G47" t="e">
-        <f t="shared" ref="G47:G51" si="42">1/0</f>
+        <f t="shared" ref="G47" si="47">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H47" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="48" spans="1:8">
+      <c r="I47">
+        <f t="shared" ca="1" si="33"/>
+        <v>6.2607356956282723E-2</v>
+      </c>
+      <c r="J47">
+        <f t="shared" ca="1" si="31"/>
+        <v>5.4022391118100144E-2</v>
+      </c>
+      <c r="K47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.50695900875241107</v>
+      </c>
+      <c r="L47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.88263503895199602</v>
+      </c>
+      <c r="M47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.16079341250557444</v>
+      </c>
+      <c r="N47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.67092689013519258</v>
+      </c>
+      <c r="O47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.71196363046227429</v>
+      </c>
+      <c r="P47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.50658451511545499</v>
+      </c>
+      <c r="Q47">
+        <f t="shared" ca="1" si="31"/>
+        <v>5.002454428189762E-2</v>
+      </c>
+      <c r="R47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.21073882350085915</v>
+      </c>
+      <c r="S47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.83463838294302894</v>
+      </c>
+      <c r="T47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.82967805602835853</v>
+      </c>
+      <c r="U47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.45219517392056374</v>
+      </c>
+      <c r="V47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.80601686183117549</v>
+      </c>
+      <c r="W47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.64508783762622901</v>
+      </c>
+      <c r="X47">
+        <f t="shared" ca="1" si="31"/>
+        <v>0.56860713430604148</v>
+      </c>
+      <c r="Y47">
+        <f t="shared" ref="Y47:Z51" ca="1" si="48">RAND()</f>
+        <v>7.1155171530684291E-2</v>
+      </c>
+      <c r="Z47">
+        <f t="shared" ca="1" si="48"/>
+        <v>7.9837719143024732E-2</v>
+      </c>
+    </row>
+    <row r="48" spans="1:26">
       <c r="A48">
         <v>47</v>
       </c>
@@ -4851,15 +8271,87 @@
         <v>3.9351851851851852E-4</v>
       </c>
       <c r="G48" t="e">
-        <f t="shared" ref="G48:G51" si="43">something</f>
+        <f t="shared" ref="G48" si="49">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H48" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="49" spans="1:8">
+      <c r="I48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.121174761499383</v>
+      </c>
+      <c r="J48">
+        <f t="shared" ca="1" si="33"/>
+        <v>6.7949115409385641E-2</v>
+      </c>
+      <c r="K48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.46586130017667449</v>
+      </c>
+      <c r="L48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.84986872888958798</v>
+      </c>
+      <c r="M48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.89565523709470385</v>
+      </c>
+      <c r="N48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.51423356031314393</v>
+      </c>
+      <c r="O48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.72160326839833866</v>
+      </c>
+      <c r="P48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.46861400404638742</v>
+      </c>
+      <c r="Q48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.78306079001817264</v>
+      </c>
+      <c r="R48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.32428185908975227</v>
+      </c>
+      <c r="S48">
+        <f t="shared" ca="1" si="33"/>
+        <v>3.0504737662333081E-2</v>
+      </c>
+      <c r="T48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.55923764599436798</v>
+      </c>
+      <c r="U48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.46504179251460165</v>
+      </c>
+      <c r="V48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.81993423513526742</v>
+      </c>
+      <c r="W48">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.98992312375549707</v>
+      </c>
+      <c r="X48">
+        <f t="shared" ca="1" si="33"/>
+        <v>8.5185897935037613E-2</v>
+      </c>
+      <c r="Y48">
+        <f t="shared" ca="1" si="48"/>
+        <v>0.6699942927537379</v>
+      </c>
+      <c r="Z48">
+        <f t="shared" ca="1" si="48"/>
+        <v>0.11844691749031899</v>
+      </c>
+    </row>
+    <row r="49" spans="1:26">
       <c r="A49">
         <v>48</v>
       </c>
@@ -4876,15 +8368,87 @@
         <v>41277.156481481485</v>
       </c>
       <c r="G49" t="e">
-        <f t="shared" ref="G49:G51" si="44">"abc"+1</f>
+        <f t="shared" ref="G49" si="50">"abc"+1</f>
         <v>#VALUE!</v>
       </c>
       <c r="H49" t="b">
         <f>FALSE</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="50" spans="1:8">
+      <c r="I49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.70980982815967875</v>
+      </c>
+      <c r="J49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.82789741134622785</v>
+      </c>
+      <c r="K49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.64870734512507122</v>
+      </c>
+      <c r="L49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.52002390660822839</v>
+      </c>
+      <c r="M49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.51013066877846103</v>
+      </c>
+      <c r="N49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.87684220239340871</v>
+      </c>
+      <c r="O49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.88875322427193004</v>
+      </c>
+      <c r="P49">
+        <f t="shared" ca="1" si="33"/>
+        <v>4.5464656537644532E-2</v>
+      </c>
+      <c r="Q49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.85755124456211418</v>
+      </c>
+      <c r="R49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.71713931417650145</v>
+      </c>
+      <c r="S49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.29143080780899133</v>
+      </c>
+      <c r="T49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.9645620101628537</v>
+      </c>
+      <c r="U49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.93209004990779509</v>
+      </c>
+      <c r="V49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.86397279129456639</v>
+      </c>
+      <c r="W49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.61133660749532603</v>
+      </c>
+      <c r="X49">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.20593571693156498</v>
+      </c>
+      <c r="Y49">
+        <f t="shared" ca="1" si="48"/>
+        <v>0.14864066315162172</v>
+      </c>
+      <c r="Z49">
+        <f t="shared" ca="1" si="48"/>
+        <v>0.50674373417612506</v>
+      </c>
+    </row>
+    <row r="50" spans="1:26">
       <c r="A50">
         <v>49</v>
       </c>
@@ -4901,15 +8465,87 @@
         <v>41278</v>
       </c>
       <c r="G50" t="e">
-        <f t="shared" ref="G50:G51" si="45">1/0</f>
+        <f t="shared" ref="G50" si="51">1/0</f>
         <v>#DIV/0!</v>
       </c>
       <c r="H50" t="b">
         <f>TRUE</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="51" spans="1:8">
+      <c r="I50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.79976480379367476</v>
+      </c>
+      <c r="J50">
+        <f t="shared" ca="1" si="33"/>
+        <v>8.9203147568626573E-2</v>
+      </c>
+      <c r="K50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.37779165008573312</v>
+      </c>
+      <c r="L50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.24244011030597545</v>
+      </c>
+      <c r="M50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.20577982505127657</v>
+      </c>
+      <c r="N50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.55342228164214169</v>
+      </c>
+      <c r="O50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.62758641986327468</v>
+      </c>
+      <c r="P50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.47997819290365218</v>
+      </c>
+      <c r="Q50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.24477142545248165</v>
+      </c>
+      <c r="R50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.3295816077656798</v>
+      </c>
+      <c r="S50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.7370427591604467</v>
+      </c>
+      <c r="T50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.61474273380639033</v>
+      </c>
+      <c r="U50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.62270641748275957</v>
+      </c>
+      <c r="V50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.65286990746213724</v>
+      </c>
+      <c r="W50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.14696954039772392</v>
+      </c>
+      <c r="X50">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.15657476597615905</v>
+      </c>
+      <c r="Y50">
+        <f t="shared" ca="1" si="48"/>
+        <v>0.8656233804356761</v>
+      </c>
+      <c r="Z50">
+        <f t="shared" ca="1" si="48"/>
+        <v>0.41558770405863499</v>
+      </c>
+    </row>
+    <row r="51" spans="1:26">
       <c r="A51">
         <v>50</v>
       </c>
@@ -4926,12 +8562,84 @@
         <v>41279.666666666664</v>
       </c>
       <c r="G51" t="e">
-        <f t="shared" ref="G51" si="46">something</f>
+        <f t="shared" ref="G51" si="52">something</f>
         <v>#NAME?</v>
       </c>
       <c r="H51" t="b">
         <f>FALSE</f>
         <v>0</v>
+      </c>
+      <c r="I51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.40130524018133118</v>
+      </c>
+      <c r="J51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.5249394768118385</v>
+      </c>
+      <c r="K51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.41093784459502303</v>
+      </c>
+      <c r="L51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.21255021270057239</v>
+      </c>
+      <c r="M51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.9581462522958325</v>
+      </c>
+      <c r="N51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.36978167301051956</v>
+      </c>
+      <c r="O51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.99343978699392743</v>
+      </c>
+      <c r="P51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.79307185504638855</v>
+      </c>
+      <c r="Q51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.81371193793142382</v>
+      </c>
+      <c r="R51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.69082752183971263</v>
+      </c>
+      <c r="S51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.4547837145035587</v>
+      </c>
+      <c r="T51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.57562058143604988</v>
+      </c>
+      <c r="U51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.92076938000571185</v>
+      </c>
+      <c r="V51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.64624829396043793</v>
+      </c>
+      <c r="W51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.98103766344527898</v>
+      </c>
+      <c r="X51">
+        <f t="shared" ca="1" si="33"/>
+        <v>0.43060670171292192</v>
+      </c>
+      <c r="Y51">
+        <f t="shared" ca="1" si="48"/>
+        <v>0.48085505273473628</v>
+      </c>
+      <c r="Z51">
+        <f t="shared" ca="1" si="48"/>
+        <v>0.14525317990041087</v>
       </c>
     </row>
   </sheetData>

</xml_diff>